<commit_message>
Opdateret plan med detaljeret uge plan
</commit_message>
<xml_diff>
--- a/Tidsplan.xlsx
+++ b/Tidsplan.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\randi\OneDrive - Aarhus universitet\IKT\4. semester\PRJ4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_3A9529A271D8F144628BDA61ECC87C2FAD9D7D7C" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{2DD7AC9E-0902-4B04-B53A-161B9195F0B0}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="11_3A9529A271D8F144628BDA61ECC87C2FAD9D7D7C" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{3475E07D-4653-4CC2-80FF-8AC53FFB9F89}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6420" yWindow="2148" windowWidth="16620" windowHeight="10212" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="1" r:id="rId1"/>
+    <sheet name="Detaljeret plan" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'2020'!$A$1:$AJ$32</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="176">
   <si>
     <t>April 2020</t>
   </si>
@@ -401,13 +402,163 @@
   </si>
   <si>
     <t>SWD, DAB, SWT, GUI, NGK: sidste lektion</t>
+  </si>
+  <si>
+    <t>Ugeskema</t>
+  </si>
+  <si>
+    <t>Uge 19</t>
+  </si>
+  <si>
+    <t>8:00-10:00</t>
+  </si>
+  <si>
+    <t>10:00-12:00</t>
+  </si>
+  <si>
+    <t>12:00-14:00</t>
+  </si>
+  <si>
+    <t>14:00-16:00</t>
+  </si>
+  <si>
+    <t>Tid/Dag</t>
+  </si>
+  <si>
+    <t>Mandag</t>
+  </si>
+  <si>
+    <t>Tirsdag</t>
+  </si>
+  <si>
+    <t>Onsdag</t>
+  </si>
+  <si>
+    <t>Torsdag</t>
+  </si>
+  <si>
+    <t>Fredag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lørdag </t>
+  </si>
+  <si>
+    <t>Søndag</t>
+  </si>
+  <si>
+    <t>Uge 20</t>
+  </si>
+  <si>
+    <t>DAB undervisning</t>
+  </si>
+  <si>
+    <t>GUI undervsing</t>
+  </si>
+  <si>
+    <t>NGK undervisning</t>
+  </si>
+  <si>
+    <t>Uge 21</t>
+  </si>
+  <si>
+    <t>NGK aflevering kl 12:00</t>
+  </si>
+  <si>
+    <t>SWD undervisning</t>
+  </si>
+  <si>
+    <t>SWT undervisning</t>
+  </si>
+  <si>
+    <t>GUI aflerving denne uge</t>
+  </si>
+  <si>
+    <t>Uge 22</t>
+  </si>
+  <si>
+    <t>PRJ4 aflevering kl. 12:00</t>
+  </si>
+  <si>
+    <t>Projekt</t>
+  </si>
+  <si>
+    <t>Andre opgaver</t>
+  </si>
+  <si>
+    <t>DAB aflevering kl 8:00</t>
+  </si>
+  <si>
+    <t>Buffer Projekt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Store Bededag</t>
+  </si>
+  <si>
+    <t>(GUI undervisning)</t>
+  </si>
+  <si>
+    <t>Kristi Himmelfartsdag</t>
+  </si>
+  <si>
+    <t>Mandag (4. maj)</t>
+  </si>
+  <si>
+    <t>Tirsdag (5. maj)</t>
+  </si>
+  <si>
+    <t>Onsdag (6. maj)</t>
+  </si>
+  <si>
+    <t>Torsdag (7. maj)</t>
+  </si>
+  <si>
+    <t>Fredag (8. maj)</t>
+  </si>
+  <si>
+    <t>Mandag (11. maj)</t>
+  </si>
+  <si>
+    <t>Tirsdag (12. maj)</t>
+  </si>
+  <si>
+    <t>Onsdag (13. maj)</t>
+  </si>
+  <si>
+    <t>Torsdag (14. maj)</t>
+  </si>
+  <si>
+    <t>Fredag (15. maj)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mandag (18. maj) </t>
+  </si>
+  <si>
+    <t>Tirsdag (19. maj)</t>
+  </si>
+  <si>
+    <t>Onsdag (20. maj)</t>
+  </si>
+  <si>
+    <t>Torsdag (21. maj)</t>
+  </si>
+  <si>
+    <t>Fredag (22. maj)</t>
+  </si>
+  <si>
+    <t>Lørdag (23. maj)</t>
+  </si>
+  <si>
+    <t>Søndag (24. maj)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
@@ -429,8 +580,28 @@
       <sz val="8"/>
       <name val="Trebuchet MS"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -485,8 +656,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -575,11 +752,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -658,6 +850,54 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -667,16 +907,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -988,7 +1219,7 @@
   </sheetPr>
   <dimension ref="A1:AJ32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -1033,39 +1264,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="32" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="29" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="30"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
-      <c r="AI1" s="26"/>
-      <c r="AJ1" s="26"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="45"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="42"/>
+      <c r="AB1" s="42"/>
+      <c r="AC1" s="42"/>
+      <c r="AD1" s="42"/>
+      <c r="AE1" s="42"/>
+      <c r="AF1" s="42"/>
+      <c r="AG1" s="42"/>
+      <c r="AH1" s="42"/>
+      <c r="AI1" s="42"/>
+      <c r="AJ1" s="42"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -2267,9 +2498,9 @@
       <c r="AB32" s="12"/>
       <c r="AC32" s="11"/>
       <c r="AD32" s="11"/>
-      <c r="AE32" s="27"/>
-      <c r="AF32" s="28"/>
-      <c r="AG32" s="28"/>
+      <c r="AE32" s="43"/>
+      <c r="AF32" s="44"/>
+      <c r="AG32" s="44"/>
       <c r="AH32" s="10"/>
       <c r="AI32" s="11"/>
       <c r="AJ32" s="11"/>
@@ -2296,4 +2527,430 @@
     <brk id="18" man="1"/>
   </colBreaks>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91744AAE-7350-402C-8283-2EDA53CCE8A7}">
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="8" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" s="36"/>
+      <c r="F5" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="J5" s="33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="34"/>
+      <c r="C6" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="34"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+    </row>
+    <row r="7" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+    </row>
+    <row r="8" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+    </row>
+    <row r="11" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+    </row>
+    <row r="14" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+    </row>
+    <row r="15" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+    </row>
+    <row r="16" spans="1:10" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E16" s="36"/>
+      <c r="F16" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="27"/>
+    </row>
+    <row r="20" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" s="37"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+    </row>
+    <row r="23" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+    </row>
+    <row r="24" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="37"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+    </row>
+    <row r="25" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="37"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+    </row>
+    <row r="28" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="F29" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="G29" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="H29" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="K29" s="27" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+    </row>
+    <row r="31" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+    </row>
+    <row r="32" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="E32" s="28"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+    </row>
+    <row r="33" spans="1:8" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>